<commit_message>
[fix] citaion theo db moi
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/Download/Citation.xlsx
+++ b/MANAGER/Excel_template/Download/Citation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>STT</t>
   </si>
@@ -42,22 +42,13 @@
     <t>Số tiền (VNĐ)</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>fe001</t>
+    <t>Trần Thị Thúy Nguyên</t>
+  </si>
+  <si>
+    <t>He130020</t>
   </si>
   <si>
     <t>FPTUHN</t>
-  </si>
-  <si>
-    <t>Kiều Quốc Tuấn</t>
-  </si>
-  <si>
-    <t>HE130002</t>
-  </si>
-  <si>
-    <t>FPTUHCM</t>
   </si>
   <si>
     <t>Số lượng trích dẫn trên Scopus</t>
@@ -432,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -446,19 +437,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="F2" s="0">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
@@ -475,10 +466,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="0">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="F3" s="0">
-        <v>9</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -536,7 +527,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="4">
-        <v>10000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="3">
@@ -544,16 +535,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[fix] citaion theo db moi (#1216)
Co-authored-by: thang1160 <35557579+thang1160@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/Download/Citation.xlsx
+++ b/MANAGER/Excel_template/Download/Citation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>STT</t>
   </si>
@@ -42,22 +42,13 @@
     <t>Số tiền (VNĐ)</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>fe001</t>
+    <t>Trần Thị Thúy Nguyên</t>
+  </si>
+  <si>
+    <t>He130020</t>
   </si>
   <si>
     <t>FPTUHN</t>
-  </si>
-  <si>
-    <t>Kiều Quốc Tuấn</t>
-  </si>
-  <si>
-    <t>HE130002</t>
-  </si>
-  <si>
-    <t>FPTUHCM</t>
   </si>
   <si>
     <t>Số lượng trích dẫn trên Scopus</t>
@@ -432,13 +423,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -446,19 +437,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="F2" s="0">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
@@ -475,10 +466,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="0">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="F3" s="0">
-        <v>9</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -536,7 +527,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="4">
-        <v>10000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="3">
@@ -544,16 +535,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>